<commit_message>
more data cleaning to add in more effect sizes from shared longevity column.
</commit_message>
<xml_diff>
--- a/Data/extra_reproduction_traits.xlsx
+++ b/Data/extra_reproduction_traits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ff242\Documents\GitHub\Thermal_Fertility_Meta-Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C6C8B3-9623-4EA8-AEF0-038E7A0A6CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E95184E-1D80-4543-A0E7-B660022BE64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A94467-3E9A-4A38-8CB1-DB69E768636C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="159">
   <si>
     <t>Status</t>
   </si>
@@ -486,6 +486,33 @@
   </si>
   <si>
     <t>Number of viable eggs</t>
+  </si>
+  <si>
+    <t>TEMP638</t>
+  </si>
+  <si>
+    <t>20B</t>
+  </si>
+  <si>
+    <t>Gharibi, M. R.et al.</t>
+  </si>
+  <si>
+    <t>Life Cycle of the Fairy Shrimp, Phallocryptus spinosa Milne Edwards, 1840 (Crustacea: Anostraca) at Different Temperatures</t>
+  </si>
+  <si>
+    <t>Phallocryptus spinosa</t>
+  </si>
+  <si>
+    <t>Thamnocephalidae</t>
+  </si>
+  <si>
+    <t>TEMP638_1</t>
+  </si>
+  <si>
+    <t>TEMP638_A</t>
+  </si>
+  <si>
+    <t>number of clutch per female</t>
   </si>
 </sst>
 </file>
@@ -534,10 +561,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -853,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B29CE22-9985-490B-AE79-57562EEB6815}">
-  <dimension ref="A1:AN43"/>
+  <dimension ref="A1:AO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4765,7 +4795,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -4887,7 +4917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -5009,7 +5039,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -5131,7 +5161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -5253,7 +5283,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -5375,7 +5405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -5497,7 +5527,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -5619,7 +5649,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -5741,7 +5771,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -5863,7 +5893,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -5985,7 +6015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -6105,6 +6135,381 @@
       </c>
       <c r="AN43" s="1" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="1">
+        <v>582</v>
+      </c>
+      <c r="D44" s="1">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI44" s="3">
+        <v>25</v>
+      </c>
+      <c r="AJ44" s="1">
+        <v>-2.2975181029999998</v>
+      </c>
+      <c r="AK44" s="1">
+        <v>0.20747795999999999</v>
+      </c>
+      <c r="AL44" s="1">
+        <v>-10</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>25</v>
+      </c>
+      <c r="AN44" s="1">
+        <v>15</v>
+      </c>
+      <c r="AO44" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="1">
+        <v>582</v>
+      </c>
+      <c r="D45" s="1">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI45" s="3">
+        <v>25</v>
+      </c>
+      <c r="AJ45" s="1">
+        <v>0.17083727600000001</v>
+      </c>
+      <c r="AK45" s="1">
+        <v>0.125456022</v>
+      </c>
+      <c r="AL45" s="1">
+        <v>-5</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>25</v>
+      </c>
+      <c r="AN45" s="1">
+        <v>20</v>
+      </c>
+      <c r="AO45" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="1">
+        <v>582</v>
+      </c>
+      <c r="D46" s="1">
+        <v>10</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI46" s="3">
+        <v>25</v>
+      </c>
+      <c r="AJ46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>25</v>
+      </c>
+      <c r="AN46" s="1">
+        <v>25</v>
+      </c>
+      <c r="AO46" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>